<commit_message>
LM35 tabela, falta o -5 e arrumar o de 5
</commit_message>
<xml_diff>
--- a/medicoes instrumed.xlsx
+++ b/medicoes instrumed.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27204"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/WESLEY/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Cloreto de magnesio(MgCl2) (20C-33humid)</t>
   </si>
@@ -39,6 +34,15 @@
   </si>
   <si>
     <t>Hidroxido de potassio (KOH)(20C</t>
+  </si>
+  <si>
+    <t>Incerteza tipo B</t>
+  </si>
+  <si>
+    <t>Incerteza tipo A</t>
+  </si>
+  <si>
+    <t>σ v</t>
   </si>
 </sst>
 </file>
@@ -145,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -180,7 +184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -357,7 +361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -365,22 +369,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="42.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
     <col min="5" max="5" width="42.33203125" customWidth="1"/>
     <col min="7" max="7" width="42.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="19">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -393,8 +399,17 @@
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="C2">
         <v>76.599999999999994</v>
       </c>
@@ -402,7 +417,7 @@
         <v>61.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="C3">
         <v>75.7</v>
       </c>
@@ -410,7 +425,7 @@
         <v>62.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="C4">
         <v>75</v>
       </c>
@@ -418,7 +433,7 @@
         <v>62.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="C5">
         <v>77.3</v>
       </c>
@@ -428,5 +443,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tabela calculando incertezas - a conferir
</commit_message>
<xml_diff>
--- a/medicoes instrumed.xlsx
+++ b/medicoes instrumed.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Cloreto de magnesio(MgCl2) (20C-33humid)</t>
   </si>
@@ -42,14 +42,53 @@
     <t>Incerteza tipo A</t>
   </si>
   <si>
-    <t>σ v</t>
+    <t>σ dht</t>
+  </si>
+  <si>
+    <t>Incerteza B temperatura</t>
+  </si>
+  <si>
+    <t>Incerteza B umidade</t>
+  </si>
+  <si>
+    <t>∆temp</t>
+  </si>
+  <si>
+    <t>∆UR</t>
+  </si>
+  <si>
+    <t>MgCl2</t>
+  </si>
+  <si>
+    <t>NaCl</t>
+  </si>
+  <si>
+    <t>Ca(NO3)2</t>
+  </si>
+  <si>
+    <t>KOH</t>
+  </si>
+  <si>
+    <t>MÉDIA</t>
+  </si>
+  <si>
+    <t>SAIS</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>∂dht /umidade media</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -58,9 +97,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -81,22 +130,268 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="35">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -104,6 +399,69 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G1:L5" totalsRowShown="0">
+  <autoFilter ref="G1:L5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="SAIS"/>
+    <tableColumn id="2" name="Média" dataDxfId="9">
+      <calculatedColumnFormula>C6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Incerteza tipo B">
+      <calculatedColumnFormula>SQRT($H$10^2 + ($J$10/$K$10)^2 *$I$10^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Incerteza tipo A" dataDxfId="2"/>
+    <tableColumn id="5" name="σ dht" dataDxfId="1">
+      <calculatedColumnFormula>SQRT(Table1[[#This Row],[Incerteza tipo B]]^2+Table1[[#This Row],[Incerteza tipo A]]^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="∂dht /umidade media" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[σ dht]]/Table1[[#This Row],[Média]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H9:K10" totalsRowShown="0">
+  <autoFilter ref="H9:K10"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Incerteza B umidade">
+      <calculatedColumnFormula>2/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Incerteza B temperatura">
+      <calculatedColumnFormula>0.5/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="∆UR"/>
+    <tableColumn id="4" name="∆temp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
+  <autoFilter ref="A1:A2"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name=" " dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B1:E5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="B1:E5"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Cloreto de magnesio(MgCl2) (20C-33humid)" dataDxfId="8"/>
+    <tableColumn id="2" name="Cloreto de Sodio(NaCl)(20C-75,3humid)" dataDxfId="7"/>
+    <tableColumn id="3" name="Nitrato de cálcio (Ca(NO3)2)(20C-56humid)" dataDxfId="6"/>
+    <tableColumn id="4" name="Hidroxido de potassio (KOH)(20C" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,80 +727,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="8" width="42" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
     <col min="11" max="11" width="16.5" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="D2" s="1">
+        <v>61.8</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <f>B7</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>SQRT($H$10^2 + ($J$10/$K$10)^2 *$I$10^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J2" t="e">
+        <f>SQRT(((B2^H2)^2+(B3-H2)^2+(B4-H2)^2+(B5-H2)^2)/3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K2" t="e">
+        <f>SQRT(Table1[[#This Row],[Incerteza tipo B]]^2+Table1[[#This Row],[Incerteza tipo A]]^2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L2" t="e">
+        <f>Table1[[#This Row],[σ dht]]/Table1[[#This Row],[Média]]</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>75.7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>62.6</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H2:H5" si="0">C7</f>
+        <v>76.150000000000006</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I5" si="1">SQRT($H$10^2 + ($J$10/$K$10)^2 *$I$10^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J3">
+        <f>SQRT(((C2^H3)^2+(C3-H3)^2+(C4-H3)^2+(C5-H3)^2)/3)</f>
+        <v>1.7597873040347751E+143</v>
+      </c>
+      <c r="K3">
+        <f>SQRT(Table1[[#This Row],[Incerteza tipo B]]^2+Table1[[#This Row],[Incerteza tipo A]]^2)</f>
+        <v>1.7597873040347751E+143</v>
+      </c>
+      <c r="L3">
+        <f>Table1[[#This Row],[σ dht]]/Table1[[#This Row],[Média]]</f>
+        <v>2.3109485279511163E+141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>75</v>
+      </c>
+      <c r="D4" s="1">
+        <v>62.6</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <f>D7</f>
+        <v>61.35</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J4">
+        <f>SQRT(((D2^H4)^2+(D3-H4)^2+(D4-H4)^2+(D5-H4)^2)/3)</f>
+        <v>4.3509322355347483E+109</v>
+      </c>
+      <c r="K4">
+        <f>SQRT(Table1[[#This Row],[Incerteza tipo B]]^2+Table1[[#This Row],[Incerteza tipo A]]^2)</f>
+        <v>4.3509322355347483E+109</v>
+      </c>
+      <c r="L4">
+        <f>Table1[[#This Row],[σ dht]]/Table1[[#This Row],[Média]]</f>
+        <v>7.0919840840012193E+107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>77.3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>58.4</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J5" t="e">
+        <f>SQRT(((E2^H5)^2+(E3-H5)^2+(E4-H5)^2+(E5-H5)^2)/3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K5" t="e">
+        <f>SQRT(Table1[[#This Row],[Incerteza tipo B]]^2+Table1[[#This Row],[Incerteza tipo A]]^2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L5" t="e">
+        <f>Table1[[#This Row],[σ dht]]/Table1[[#This Row],[Média]]</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <f>(B2+B3+B4+B5)/4</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>(C2+C3+C4+C5)/4</f>
+        <v>76.150000000000006</v>
+      </c>
+      <c r="D7" s="1">
+        <f>(D2+D3+D4+D5)/4</f>
+        <v>61.35</v>
+      </c>
+      <c r="E7" s="1">
+        <f>(E2+E3+E4+E5)/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="H10">
+        <f>2/2</f>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f>0.5/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="J10">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="C2">
-        <v>76.599999999999994</v>
-      </c>
-      <c r="E2">
-        <v>61.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="C3">
-        <v>75.7</v>
-      </c>
-      <c r="E3">
-        <v>62.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="C4">
-        <v>75</v>
-      </c>
-      <c r="E4">
-        <v>62.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="C5">
-        <v>77.3</v>
-      </c>
-      <c r="E5">
-        <v>58.4</v>
+      <c r="K10">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>